<commit_message>
exploring data structure and printing
</commit_message>
<xml_diff>
--- a/xlsx-files/fromThis.xlsx
+++ b/xlsx-files/fromThis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afrok\Documents\Google Drive\GoingPro\Software Development\Python\Python-myShit\files-and-python\xlsx-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160F98AE-5E39-4376-B152-40B09EDA7550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6FEE8C-9FCF-4185-95F8-2A405891E583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="16608" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -395,7 +395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -437,7 +437,7 @@
         <v>44642</v>
       </c>
       <c r="D7">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -451,7 +451,7 @@
         <v>44643</v>
       </c>
       <c r="D8">
-        <v>1032</v>
+        <v>1034</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -465,7 +465,7 @@
         <v>44644</v>
       </c>
       <c r="D9">
-        <v>1032</v>
+        <v>1035</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -479,7 +479,7 @@
         <v>44645</v>
       </c>
       <c r="D10">
-        <v>1032</v>
+        <v>1036</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -493,7 +493,7 @@
         <v>44646</v>
       </c>
       <c r="D11">
-        <v>1032</v>
+        <v>1037</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -507,7 +507,7 @@
         <v>44647</v>
       </c>
       <c r="D12">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="E12" t="s">
         <v>12</v>
@@ -538,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E9F203C-6216-4BD7-B3A8-4D3A6FD9AB4E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>